<commit_message>
Updated lynx density csv and excel with proper winter column
</commit_message>
<xml_diff>
--- a/data/Lynx Density_simple.xlsx
+++ b/data/Lynx Density_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamg\Documents\M.Sc\Hare HR paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89DF90B-8CE6-41E8-873D-CAD5DEA6CF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F27BE57-A8D3-461B-BE91-DFA847FE1E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="1725" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lynx Density_simple" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
-    <t>Season</t>
-  </si>
-  <si>
     <t>mean.tracks.pertracknight.per100km</t>
   </si>
   <si>
@@ -46,115 +43,118 @@
     <t>dens.estimate.per100km2</t>
   </si>
   <si>
-    <t>87/88</t>
-  </si>
-  <si>
-    <t>88/89</t>
-  </si>
-  <si>
-    <t>89/90</t>
-  </si>
-  <si>
-    <t>90/91</t>
-  </si>
-  <si>
-    <t>91/92</t>
-  </si>
-  <si>
-    <t>92/93</t>
-  </si>
-  <si>
-    <t>93/94</t>
-  </si>
-  <si>
-    <t>94/95</t>
-  </si>
-  <si>
-    <t>95/96</t>
-  </si>
-  <si>
-    <t>96/97</t>
-  </si>
-  <si>
-    <t>97/98</t>
-  </si>
-  <si>
-    <t>98/99</t>
-  </si>
-  <si>
-    <t>99/00</t>
-  </si>
-  <si>
-    <t>00/01</t>
-  </si>
-  <si>
-    <t>13/14</t>
-  </si>
-  <si>
-    <t>14/15</t>
-  </si>
-  <si>
-    <t>15/16</t>
-  </si>
-  <si>
-    <t>16/17</t>
-  </si>
-  <si>
-    <t>17/18</t>
-  </si>
-  <si>
-    <t>18/19</t>
-  </si>
-  <si>
-    <t>19/20</t>
-  </si>
-  <si>
-    <t>20/21</t>
-  </si>
-  <si>
-    <t>21/22</t>
-  </si>
-  <si>
-    <t>01/02</t>
-  </si>
-  <si>
-    <t>02/03</t>
-  </si>
-  <si>
-    <t>03/04</t>
-  </si>
-  <si>
-    <t>04/05</t>
-  </si>
-  <si>
-    <t>05/06</t>
-  </si>
-  <si>
-    <t>06/07</t>
-  </si>
-  <si>
-    <t>07/08</t>
-  </si>
-  <si>
-    <t>08/09</t>
-  </si>
-  <si>
-    <t>09/10</t>
-  </si>
-  <si>
-    <t>10/11</t>
-  </si>
-  <si>
-    <t>11/12</t>
-  </si>
-  <si>
-    <t>12/13</t>
-  </si>
-  <si>
     <t>Lower 95% for graph</t>
   </si>
   <si>
     <t>Upper 95% for graph</t>
+  </si>
+  <si>
+    <t>1987-1988</t>
+  </si>
+  <si>
+    <t>1988-1989</t>
+  </si>
+  <si>
+    <t>1989-1990</t>
+  </si>
+  <si>
+    <t>1990-1991</t>
+  </si>
+  <si>
+    <t>1991-1992</t>
+  </si>
+  <si>
+    <t>1992-1993</t>
+  </si>
+  <si>
+    <t>1993-1994</t>
+  </si>
+  <si>
+    <t>1994-1995</t>
+  </si>
+  <si>
+    <t>1995-1996</t>
+  </si>
+  <si>
+    <t>1996-1997</t>
+  </si>
+  <si>
+    <t>1997-1998</t>
+  </si>
+  <si>
+    <t>1998-1999</t>
+  </si>
+  <si>
+    <t>1999-2000</t>
+  </si>
+  <si>
+    <t>2000-2001</t>
+  </si>
+  <si>
+    <t>2001-2002</t>
+  </si>
+  <si>
+    <t>2002-2003</t>
+  </si>
+  <si>
+    <t>2003-2004</t>
+  </si>
+  <si>
+    <t>2004-2005</t>
+  </si>
+  <si>
+    <t>2005-2006</t>
+  </si>
+  <si>
+    <t>2006-2007</t>
+  </si>
+  <si>
+    <t>2007-2008</t>
+  </si>
+  <si>
+    <t>2008-2009</t>
+  </si>
+  <si>
+    <t>2009-2010</t>
+  </si>
+  <si>
+    <t>2010-2011</t>
+  </si>
+  <si>
+    <t>2011-2012</t>
+  </si>
+  <si>
+    <t>2012-2013</t>
+  </si>
+  <si>
+    <t>2013-2014</t>
+  </si>
+  <si>
+    <t>2014-2015</t>
+  </si>
+  <si>
+    <t>2015-2016</t>
+  </si>
+  <si>
+    <t>2016-2017</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>2019-2020</t>
+  </si>
+  <si>
+    <t>2020-2021</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>winter</t>
   </si>
 </sst>
 </file>
@@ -162,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -306,16 +306,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -641,7 +642,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -686,51 +687,43 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="44" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -768,9 +761,8 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Coyote" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal_Lynx Tracks" xfId="43" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal_Sheet1" xfId="44" xr:uid="{7B0EA98F-9A99-493D-9F0D-A1C4CA2DAE95}"/>
+    <cellStyle name="Normal_Lynx Tracks" xfId="42" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="43" xr:uid="{7B0EA98F-9A99-493D-9F0D-A1C4CA2DAE95}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1090,47 +1082,47 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="33.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
         <v>7.9177999999999997</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="6">
         <v>0.87419999999999998</v>
       </c>
       <c r="D2">
@@ -1144,13 +1136,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
         <v>13.854900000000001</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="6">
         <v>1.2083999999999999</v>
       </c>
       <c r="D3">
@@ -1164,13 +1156,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
         <v>22.400200000000002</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <v>2.3847999999999998</v>
       </c>
       <c r="D4">
@@ -1184,13 +1176,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
         <v>53.887799999999999</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <v>4.1262999999999996</v>
       </c>
       <c r="D5">
@@ -1204,13 +1196,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
         <v>35.796199999999999</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
         <v>2.8344</v>
       </c>
       <c r="D6">
@@ -1224,13 +1216,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
         <v>13.776300000000001</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="6">
         <v>1.6721999999999999</v>
       </c>
       <c r="D7">
@@ -1244,13 +1236,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
         <v>4.5732999999999997</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="6">
         <v>0.96989999999999998</v>
       </c>
       <c r="D8">
@@ -1264,13 +1256,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
         <v>10.519600000000001</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="6">
         <v>2.1564999999999999</v>
       </c>
       <c r="D9">
@@ -1284,13 +1276,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="6">
+      <c r="A10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
         <v>14.792</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>1.8681000000000001</v>
       </c>
       <c r="D10">
@@ -1304,13 +1296,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6">
+      <c r="A11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
         <v>27.250599999999999</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="6">
         <v>3.8881000000000001</v>
       </c>
       <c r="D11">
@@ -1324,13 +1316,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6">
+      <c r="A12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
         <v>53.866</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="6">
         <v>6.9333999999999998</v>
       </c>
       <c r="D12">
@@ -1344,13 +1336,13 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6">
+      <c r="A13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
         <v>82.414000000000001</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="6">
         <v>8.7797000000000001</v>
       </c>
       <c r="D13">
@@ -1364,13 +1356,13 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="6">
+      <c r="A14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
         <v>72.6751</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="6">
         <v>6.3</v>
       </c>
       <c r="D14">
@@ -1384,13 +1376,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="6">
+      <c r="A15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
         <v>2.6187999999999998</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="6">
         <v>0.72440000000000004</v>
       </c>
       <c r="D15">
@@ -1404,13 +1396,13 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="6">
+      <c r="A16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
         <v>2.8898999999999999</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="6">
         <v>0.83220000000000005</v>
       </c>
       <c r="D16">
@@ -1424,13 +1416,13 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="6">
+      <c r="A17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
         <v>5.3647999999999998</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="6">
         <v>1.0763</v>
       </c>
       <c r="D17">
@@ -1444,13 +1436,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="6">
+      <c r="A18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
         <v>6.3826999999999998</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="6">
         <v>1.4721</v>
       </c>
       <c r="D18">
@@ -1464,13 +1456,13 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="6">
+      <c r="A19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
         <v>11.432499999999999</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="6">
         <v>1.8461000000000001</v>
       </c>
       <c r="D19">
@@ -1484,13 +1476,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="6">
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
         <v>21.5947</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="6">
         <v>3.6404000000000001</v>
       </c>
       <c r="D20">
@@ -1504,13 +1496,13 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="7">
+      <c r="A21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3">
         <v>39.363</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="7">
         <v>5.4669999999999996</v>
       </c>
       <c r="D21">
@@ -1524,13 +1516,13 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="7">
+      <c r="A22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3">
         <v>16.241</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="7">
         <v>3.9159999999999999</v>
       </c>
       <c r="D22">
@@ -1544,13 +1536,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="8">
+      <c r="A23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4">
         <v>21.343</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="8">
         <v>3.4529999999999998</v>
       </c>
       <c r="D23">
@@ -1564,13 +1556,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="9">
+      <c r="A24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="5">
         <v>21.981999999999999</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="9">
         <v>3.2240000000000002</v>
       </c>
       <c r="D24">
@@ -1584,13 +1576,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="9">
+      <c r="A25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="5">
         <v>15.965</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="9">
         <v>2.621</v>
       </c>
       <c r="D25">
@@ -1604,13 +1596,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="9">
+      <c r="A26" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="5">
         <v>14.31</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="10">
         <v>2.6890000000000001</v>
       </c>
       <c r="D26">
@@ -1624,13 +1616,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="9">
+      <c r="A27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="5">
         <v>18.722999999999999</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="11">
         <v>3.6070000000000002</v>
       </c>
       <c r="D27">
@@ -1644,13 +1636,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="9">
+      <c r="A28" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="5">
         <v>16.5</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="11">
         <v>3.7890000000000001</v>
       </c>
       <c r="D28">
@@ -1664,13 +1656,13 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="9">
+      <c r="A29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="5">
         <v>38.340000000000003</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="11">
         <v>5.9370000000000003</v>
       </c>
       <c r="D29">
@@ -1684,13 +1676,13 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="9">
+      <c r="A30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="5">
         <v>30.969000000000001</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="11">
         <v>4.6479999999999997</v>
       </c>
       <c r="D30">
@@ -1704,13 +1696,13 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="9">
+      <c r="A31" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="5">
         <v>59.874000000000002</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="11">
         <v>6.4240000000000004</v>
       </c>
       <c r="D31">
@@ -1724,13 +1716,13 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="9">
+      <c r="A32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="5">
         <v>59.670999999999999</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="11">
         <v>8.2319999999999993</v>
       </c>
       <c r="D32">
@@ -1744,13 +1736,13 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="9">
+      <c r="A33" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="5">
         <v>28.969000000000001</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="11">
         <v>5.3810000000000002</v>
       </c>
       <c r="D33">
@@ -1764,13 +1756,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="9">
+      <c r="A34" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="5">
         <v>27.628</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="11">
         <v>3</v>
       </c>
       <c r="D34">
@@ -1784,13 +1776,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="9">
+      <c r="A35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="5">
         <v>24.440999999999999</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="11">
         <v>6.6390000000000002</v>
       </c>
       <c r="D35">
@@ -1804,13 +1796,13 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="9">
+      <c r="A36" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="5">
         <v>1.907</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="11">
         <v>0.92600000000000005</v>
       </c>
       <c r="D36">
@@ -1824,6 +1816,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>